<commit_message>
Exam Week 1st commit
</commit_message>
<xml_diff>
--- a/WebAlap/webfejlesztes_iranyelvek_v2024252_v2.xlsx
+++ b/WebAlap/webfejlesztes_iranyelvek_v2024252_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PatrikITWorkSpace\Elte_24_25_2\WebAlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F61EDA7-C1E3-416D-B283-DF3237A915A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC6F829-A969-4277-8012-2045B2D7FFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="25580" windowHeight="15260" activeTab="1" xr2:uid="{1BD8638E-000E-4472-8AE1-C32ECD41C6A4}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="25580" windowHeight="15260" xr2:uid="{1BD8638E-000E-4472-8AE1-C32ECD41C6A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
   <si>
     <t>Neved:</t>
   </si>
@@ -614,6 +614,15 @@
   </si>
   <si>
     <t>Mind</t>
+  </si>
+  <si>
+    <t>Bartók Patrik Róbert</t>
+  </si>
+  <si>
+    <t>MNDJ3P</t>
+  </si>
+  <si>
+    <t>mndj3p@inf.elte.hu, bartokpatrikrobert@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1500,40 +1509,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1541,6 +1516,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1557,6 +1535,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1587,6 +1568,34 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3590,8 +3599,8 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3612,15 +3621,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="66"/>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
       <c r="I1" s="66"/>
       <c r="J1" s="68" t="s">
         <v>99</v>
@@ -3631,12 +3640,14 @@
       <c r="B2" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
+      <c r="C2" s="119" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
       <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
@@ -3644,12 +3655,14 @@
       <c r="B3" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
+      <c r="C3" s="119" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
       <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
@@ -3657,52 +3670,54 @@
       <c r="B4" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
+      <c r="C4" s="119" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
       <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="65"/>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
       <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="65"/>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
       <c r="I6" s="65"/>
     </row>
     <row r="7" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="65"/>
-      <c r="B7" s="112" t="str">
+      <c r="B7" s="102" t="str">
         <f>CONCATENATE("Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább ",D12," pontot el kell érni. A hallgatói és tutori értékelés tekintetében, maximum 15 darab irányelvben lehet eltérés, ennél több esetén már nem tudjuk elfogadni a feladatot.")</f>
         <v>Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább 50 pontot el kell érni. A hallgatói és tutori értékelés tekintetében, maximum 15 darab irányelvben lehet eltérés, ennél több esetén már nem tudjuk elfogadni a feladatot.</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
       <c r="I7" s="65"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -3740,11 +3755,11 @@
         <v>47</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="103" t="s">
+      <c r="F10" s="121" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
       <c r="I10" s="65"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -3758,9 +3773,9 @@
         <v>100</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
       <c r="I11" s="65"/>
     </row>
     <row r="12" spans="1:10" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3773,9 +3788,9 @@
         <v>50</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
       <c r="I12" s="65"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -3818,12 +3833,12 @@
         <v>100</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="100" t="str">
+      <c r="F15" s="106" t="str">
         <f>CONCATENATE("Ha a feladatot önállóan értékelnénk, akkor az önértékelésed alapján ",VLOOKUP(D15,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
         <v>Ha a feladatot önállóan értékelnénk, akkor az önértékelésed alapján jeles  érdemjegyet kapnál rá.</v>
       </c>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
       <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3850,11 +3865,11 @@
         <v>Még nincs adat.</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="117" t="s">
+      <c r="F17" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="118"/>
-      <c r="H17" s="119"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="110"/>
       <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3868,9 +3883,9 @@
         <v>Még nincs adat.</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="121"/>
-      <c r="H18" s="122"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="113"/>
       <c r="I18" s="65"/>
     </row>
     <row r="19" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3884,9 +3899,9 @@
         <v>Még nincs adat.</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="124"/>
-      <c r="H19" s="125"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="116"/>
       <c r="I19" s="65"/>
     </row>
     <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -3912,11 +3927,11 @@
         <v>20</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="100" t="s">
+      <c r="F21" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
       <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3929,25 +3944,25 @@
         <v>10</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="107"/>
       <c r="I22" s="65"/>
     </row>
     <row r="23" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="65"/>
-      <c r="B23" s="114" t="s">
+      <c r="B23" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="115"/>
+      <c r="C23" s="105"/>
       <c r="D23" s="44" t="str">
         <f>IF(D26=TRUE,SUM(Irányelvek!L2:L48),"Még nincs adat.")</f>
         <v>Még nincs adat.</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
       <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3961,9 +3976,9 @@
         <v>Még nincs adat.</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="107"/>
       <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3979,10 +3994,10 @@
     </row>
     <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="65"/>
-      <c r="B26" s="109" t="s">
+      <c r="B26" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="109"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="45" t="b">
         <v>0</v>
       </c>
@@ -3994,10 +4009,10 @@
     </row>
     <row r="27" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="65"/>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="107"/>
+      <c r="C27" s="125"/>
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
@@ -4007,10 +4022,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="65"/>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="98"/>
+      <c r="C28" s="118"/>
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
       <c r="F28" s="46"/>
@@ -4020,13 +4035,13 @@
     </row>
     <row r="29" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="65"/>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="97"/>
       <c r="I29" s="65"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -4043,17 +4058,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Mz7EfEDe6v8cDUz4TxEHDWHiqsbUlOKtpPmMASCpJrCgqIKcchwB59qyedMGM9nhDxctmLUFNc/7+3pzDxMfOQ==" saltValue="ufiuVYYMa4lem5kpeJ7gNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F21:H24"/>
-    <mergeCell ref="F17:H19"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B12:C12"/>
@@ -4070,6 +4074,17 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F21:H24"/>
+    <mergeCell ref="F17:H19"/>
   </mergeCells>
   <conditionalFormatting sqref="D15">
     <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
@@ -4130,7 +4145,7 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>

</xml_diff>